<commit_message>
bugging in add daumuc
</commit_message>
<xml_diff>
--- a/data/data thẻ việc.xlsx
+++ b/data/data thẻ việc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="262">
   <si>
     <t>STT</t>
   </si>
@@ -546,7 +546,7 @@
     <t>Tất cả</t>
   </si>
   <si>
-    <t xml:space="preserve">Phan Duy Dương </t>
+    <t>Phan Duy Dương</t>
   </si>
   <si>
     <t>Hồ Gia Bảo bí thư</t>
@@ -588,9 +588,6 @@
     <t>Phạm Trường Giang</t>
   </si>
   <si>
-    <t>Phan Duy Dương</t>
-  </si>
-  <si>
     <t xml:space="preserve">Đầu mục1 </t>
   </si>
   <si>
@@ -675,7 +672,7 @@
     <t>Ngày</t>
   </si>
   <si>
-    <t>Phùng Tuấn Kiệt</t>
+    <t>Phạm Hoàng Doanh</t>
   </si>
   <si>
     <t xml:space="preserve">Quý </t>
@@ -4556,7 +4553,7 @@
       <c r="D4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="15" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4845,7 +4842,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -4881,7 +4878,7 @@
         <v>12</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -4899,7 +4896,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -5898,7 +5895,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="C2" sqref="C2" pane="topRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
@@ -5921,54 +5921,54 @@
         <v>41</v>
       </c>
       <c r="C1" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="28" t="s">
         <v>191</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>192</v>
       </c>
       <c r="F1" s="23"/>
       <c r="G1" s="24"/>
       <c r="H1" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="I1" s="27" t="s">
-        <v>194</v>
-      </c>
       <c r="J1" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K1" s="23"/>
       <c r="L1" s="24"/>
       <c r="M1" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="N1" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="N1" s="27" t="s">
-        <v>196</v>
-      </c>
       <c r="O1" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P1" s="23"/>
       <c r="Q1" s="24"/>
       <c r="R1" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="S1" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="27" t="s">
-        <v>198</v>
-      </c>
       <c r="T1" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U1" s="23"/>
       <c r="V1" s="24"/>
       <c r="W1" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="X1" s="27" t="s">
         <v>199</v>
-      </c>
-      <c r="X1" s="27" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -5977,46 +5977,46 @@
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
       <c r="E2" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="27" t="s">
         <v>202</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>203</v>
       </c>
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
       <c r="J2" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="L2" s="27" t="s">
         <v>202</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>203</v>
       </c>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
       <c r="O2" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="P2" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="P2" s="27" t="s">
-        <v>202</v>
-      </c>
       <c r="Q2" s="27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="R2" s="29"/>
       <c r="S2" s="29"/>
       <c r="T2" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="U2" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="U2" s="27" t="s">
+      <c r="V2" s="27" t="s">
         <v>202</v>
-      </c>
-      <c r="V2" s="27" t="s">
-        <v>203</v>
       </c>
       <c r="W2" s="29"/>
       <c r="X2" s="29"/>
@@ -6029,28 +6029,28 @@
         <v>54</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>206</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>207</v>
       </c>
       <c r="F3" s="30">
         <v>3.0</v>
       </c>
       <c r="G3" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="I3" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="J3" s="30" t="s">
         <v>210</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>211</v>
       </c>
       <c r="K3" s="30">
         <v>1.0</v>
@@ -6059,19 +6059,19 @@
         <v>98</v>
       </c>
       <c r="M3" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="N3" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="O3" s="30" t="s">
         <v>213</v>
-      </c>
-      <c r="O3" s="30" t="s">
-        <v>214</v>
       </c>
       <c r="P3" s="30">
         <v>6.0</v>
       </c>
       <c r="Q3" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R3" s="31"/>
       <c r="S3" s="31"/>
@@ -6090,13 +6090,13 @@
         <v>63</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="F4" s="30">
         <v>10.0</v>
@@ -6105,24 +6105,24 @@
         <v>75</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="K4" s="30">
         <v>10.0</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M4" s="31"/>
       <c r="N4" s="31"/>
-      <c r="O4" s="30" t="s">
-        <v>211</v>
+      <c r="O4" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="P4" s="30"/>
       <c r="Q4" s="30"/>
@@ -6143,13 +6143,13 @@
         <v>69</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="F5" s="30">
         <v>6.0</v>
@@ -6158,24 +6158,24 @@
         <v>75</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="K5" s="30">
         <v>7.0</v>
       </c>
       <c r="L5" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M5" s="31"/>
       <c r="N5" s="31"/>
-      <c r="O5" s="30" t="s">
-        <v>214</v>
+      <c r="O5" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
@@ -6196,13 +6196,13 @@
         <v>77</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>218</v>
+        <v>209</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>181</v>
       </c>
       <c r="F6" s="30">
         <v>1.0</v>
@@ -6211,24 +6211,24 @@
         <v>75</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>218</v>
+        <v>209</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>217</v>
       </c>
       <c r="K6" s="30">
         <v>5.0</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
-      <c r="O6" s="30" t="s">
-        <v>218</v>
+      <c r="O6" s="17" t="s">
+        <v>217</v>
       </c>
       <c r="P6" s="30"/>
       <c r="Q6" s="30"/>
@@ -6249,13 +6249,13 @@
         <v>84</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>189</v>
+        <v>209</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>178</v>
       </c>
       <c r="F7" s="30">
         <v>10.0</v>
@@ -6264,13 +6264,13 @@
         <v>75</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>189</v>
+        <v>209</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>178</v>
       </c>
       <c r="K7" s="30">
         <v>6.0</v>
@@ -6280,8 +6280,8 @@
       </c>
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
-      <c r="O7" s="30" t="s">
-        <v>189</v>
+      <c r="O7" s="17" t="s">
+        <v>178</v>
       </c>
       <c r="P7" s="30"/>
       <c r="Q7" s="30"/>
@@ -6302,13 +6302,13 @@
         <v>89</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>207</v>
+        <v>209</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="F8" s="30">
         <v>9.0</v>
@@ -6317,13 +6317,13 @@
         <v>75</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>207</v>
+        <v>209</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="K8" s="30">
         <v>3.0</v>
@@ -6333,8 +6333,8 @@
       </c>
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
-      <c r="O8" s="30" t="s">
-        <v>207</v>
+      <c r="O8" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="P8" s="30"/>
       <c r="Q8" s="31"/>
@@ -6355,13 +6355,13 @@
         <v>94</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="F9" s="30">
         <v>3.0</v>
@@ -6370,13 +6370,13 @@
         <v>75</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J9" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="K9" s="30">
         <v>5.0</v>
@@ -6385,8 +6385,8 @@
         <v>75</v>
       </c>
       <c r="N9" s="31"/>
-      <c r="O9" s="30" t="s">
-        <v>211</v>
+      <c r="O9" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="P9" s="30"/>
       <c r="Q9" s="31"/>
@@ -6407,13 +6407,13 @@
         <v>100</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>181</v>
       </c>
       <c r="F10" s="30">
         <v>7.0</v>
@@ -6422,24 +6422,24 @@
         <v>75</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>181</v>
       </c>
       <c r="K10" s="30">
         <v>8.0</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M10" s="31"/>
       <c r="N10" s="31"/>
-      <c r="O10" s="30" t="s">
-        <v>214</v>
+      <c r="O10" s="17" t="s">
+        <v>181</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="31"/>
@@ -6460,13 +6460,13 @@
         <v>104</v>
       </c>
       <c r="C11" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>189</v>
+      <c r="E11" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="F11" s="30">
         <v>2.0</v>
@@ -6475,28 +6475,28 @@
         <v>98</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>189</v>
+        <v>220</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="K11" s="30">
         <v>8.0</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M11" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="N11" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="N11" s="30" t="s">
-        <v>224</v>
-      </c>
-      <c r="O11" s="30" t="s">
-        <v>189</v>
+      <c r="O11" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="P11" s="30">
         <v>1.0</v>
@@ -6521,28 +6521,28 @@
         <v>110</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>207</v>
+        <v>220</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>183</v>
       </c>
       <c r="F12" s="30">
         <v>7.0</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I12" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>183</v>
       </c>
       <c r="K12" s="30">
         <v>8.0</v>
@@ -6551,19 +6551,19 @@
         <v>98</v>
       </c>
       <c r="M12" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="N12" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="N12" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="O12" s="30" t="s">
-        <v>207</v>
+      <c r="O12" s="17" t="s">
+        <v>183</v>
       </c>
       <c r="P12" s="30">
         <v>5.0</v>
       </c>
       <c r="Q12" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R12" s="31"/>
       <c r="S12" s="31"/>
@@ -6582,43 +6582,43 @@
         <v>114</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>184</v>
       </c>
       <c r="F13" s="30">
         <v>2.0</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="J13" s="30" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>184</v>
       </c>
       <c r="K13" s="30">
         <v>4.0</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N13" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="O13" s="30" t="s">
-        <v>211</v>
+        <v>227</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>184</v>
       </c>
       <c r="P13" s="30">
         <v>8.0</v>
@@ -6643,43 +6643,43 @@
         <v>119</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>214</v>
+        <v>220</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>185</v>
       </c>
       <c r="F14" s="30">
         <v>1.0</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="J14" s="30" t="s">
-        <v>214</v>
+        <v>205</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>185</v>
       </c>
       <c r="K14" s="30">
         <v>1.0</v>
       </c>
       <c r="L14" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M14" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="O14" s="30" t="s">
-        <v>214</v>
+        <v>227</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>185</v>
       </c>
       <c r="P14" s="30">
         <v>1.0</v>
@@ -6704,28 +6704,28 @@
         <v>122</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>218</v>
+        <v>220</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="F15" s="30">
         <v>8.0</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H15" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="I15" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="I15" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="J15" s="30" t="s">
-        <v>218</v>
+      <c r="J15" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="K15" s="30">
         <v>7.0</v>
@@ -6734,13 +6734,13 @@
         <v>75</v>
       </c>
       <c r="M15" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N15" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="O15" s="30" t="s">
-        <v>218</v>
+        <v>209</v>
+      </c>
+      <c r="O15" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="P15" s="30">
         <v>4.0</v>
@@ -6765,28 +6765,28 @@
         <v>124</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="F16" s="30">
         <v>2.0</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="K16" s="30">
         <v>7.0</v>
@@ -6795,13 +6795,13 @@
         <v>75</v>
       </c>
       <c r="M16" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="O16" s="30" t="s">
-        <v>189</v>
+        <v>205</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="P16" s="30">
         <v>6.0</v>
@@ -6826,28 +6826,28 @@
         <v>127</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="F17" s="30">
         <v>6.0</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I17" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>207</v>
+        <v>209</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="K17" s="30">
         <v>5.0</v>
@@ -6856,13 +6856,13 @@
         <v>98</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N17" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="O17" s="30" t="s">
-        <v>207</v>
+        <v>212</v>
+      </c>
+      <c r="O17" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="P17" s="30">
         <v>7.0</v>
@@ -6887,13 +6887,13 @@
         <v>129</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>211</v>
+        <v>220</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>188</v>
       </c>
       <c r="F18" s="30">
         <v>9.0</v>
@@ -6902,28 +6902,28 @@
         <v>75</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>188</v>
       </c>
       <c r="K18" s="30">
         <v>2.0</v>
       </c>
       <c r="L18" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M18" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N18" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="O18" s="30" t="s">
-        <v>211</v>
+        <v>236</v>
+      </c>
+      <c r="O18" s="17" t="s">
+        <v>188</v>
       </c>
       <c r="P18" s="30">
         <v>1.0</v>
@@ -6948,13 +6948,13 @@
         <v>131</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>214</v>
+        <v>212</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="F19" s="30">
         <v>6.0</v>
@@ -6963,28 +6963,28 @@
         <v>98</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>214</v>
+        <v>205</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="K19" s="30">
         <v>1.0</v>
       </c>
       <c r="L19" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M19" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N19" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="O19" s="30" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="P19" s="30">
         <v>9.0</v>
@@ -7009,43 +7009,43 @@
         <v>132</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>218</v>
+        <v>205</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="F20" s="30">
         <v>4.0</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>218</v>
+        <v>236</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="K20" s="30">
         <v>8.0</v>
       </c>
       <c r="L20" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M20" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N20" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="O20" s="30" t="s">
-        <v>218</v>
+        <v>205</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="P20" s="30">
         <v>9.0</v>
@@ -7070,28 +7070,28 @@
         <v>134</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>189</v>
+        <v>236</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="F21" s="30">
         <v>8.0</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I21" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>189</v>
+        <v>205</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="K21" s="30">
         <v>4.0</v>
@@ -7100,19 +7100,19 @@
         <v>75</v>
       </c>
       <c r="M21" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N21" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="O21" s="30" t="s">
-        <v>189</v>
+        <v>205</v>
+      </c>
+      <c r="O21" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="P21" s="30">
         <v>10.0</v>
       </c>
       <c r="Q21" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R21" s="31"/>
       <c r="S21" s="31"/>
@@ -7131,43 +7131,43 @@
         <v>135</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>207</v>
+        <v>212</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="F22" s="30">
         <v>10.0</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="J22" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="K22" s="30">
         <v>3.0</v>
       </c>
       <c r="L22" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M22" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N22" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="O22" s="30" t="s">
-        <v>207</v>
+        <v>209</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="P22" s="30">
         <v>6.0</v>
@@ -7192,28 +7192,28 @@
         <v>137</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>211</v>
+        <v>205</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="F23" s="30">
         <v>4.0</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I23" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="J23" s="30" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="K23" s="30">
         <v>1.0</v>
@@ -7222,13 +7222,13 @@
         <v>98</v>
       </c>
       <c r="M23" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="O23" s="30" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="P23" s="30">
         <v>7.0</v>
@@ -8229,11 +8229,50 @@
     <mergeCell ref="T1:V1"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E23 J3:J23 O3:O23">
-      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O15">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Lưu Cảnh Tùng"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J6 O6">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Phạm Hoàng Doanh"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O11 O21">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Bùi Ngọc Quân,Bùi Ngọc Quân"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E8 J8 O8">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Lê Duy Dương"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O16">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Lê Minh Đức"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O13">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Vũ Văn Hiếu"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E5 J3:J5 O3:O5 O9 J9:J15 O19:O20 E9:E23 J17:J23 O22:O23">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Nguyễn Ngọc Hiệp,Nguyễn Lan Anh,Bùi Ngọc Quân,Nguyễn Hữu Đức,Vũ Văn Hiếu,Trần Thế Vinh,Lưu Cảnh Tùng,Lê Minh Đức,Phạm Trường Giang,Nguyễn Ngọc Hiệp,Bùi Ngọc Quân"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J16">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Nguyễn Ngọc Hiệp,Nguyễn Lan Anh,Bùi Ngọc Quân,Nguyễn Hữu Đức,Vũ Văn Hiếu,Trần Thế Vinh,Lưu Cảnh Tùng,Tất cả"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G23 L3:L23 Q11:Q23">
       <formula1>"Giờ,Năm,Ngày,Quý,Tháng"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E7 J7 O7">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Nguyễn Quang Huy"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O18">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Nguyễn Ngọc Hiệp,Phạm Trường Giang,Lê Minh Đức"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O14">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Trần Thế Vinh"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E6 O10">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Nguyễn Lan Anh"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O12">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Nguyễn Hữu Đức"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O17">
+      <formula1>"Lý Hoài Lâm,Nguyễn Thế Việt,Phạm Trang(3i),Phan Duy Dương,Phùng Tuấn Kiệt,Hồ Gia Bảo bí thư,Phạm Trường Giang,Lê Minh Đức"</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
khong co nhan su
</commit_message>
<xml_diff>
--- a/data/data thẻ việc.xlsx
+++ b/data/data thẻ việc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="263">
   <si>
     <t>STT</t>
   </si>
@@ -213,7 +213,7 @@
     <t>Hợp đồng sản xuất với đối tác nước ngoài</t>
   </si>
   <si>
-    <t>BETA (REACTJS-NODEJS)</t>
+    <t>BETA (REACTJS - NODEJS)</t>
   </si>
   <si>
     <t>Trung bình</t>
@@ -231,7 +231,7 @@
     <t>Hợp đồng sản xuất theo đơn đặt hàng</t>
   </si>
   <si>
-    <t>SIGMA (base.net7)</t>
+    <t>SIGMA(base.net7)</t>
   </si>
   <si>
     <t>Rất quan trọng</t>
@@ -324,7 +324,7 @@
     <t>Hợp đồng liên doanh sản xuất</t>
   </si>
   <si>
-    <t>BETA 1 (REACTJS-NODEJS)</t>
+    <t>BETA 1 (REACTJS - NODEJS)</t>
   </si>
   <si>
     <t>12,000,000</t>
@@ -336,7 +336,7 @@
     <t>Quản lý tồn kho</t>
   </si>
   <si>
-    <t>BETA 3 (REACTJS-NODEJS)</t>
+    <t>BETA 3 (REACTJS - NODEJS)</t>
   </si>
   <si>
     <t>Cao</t>
@@ -354,7 +354,7 @@
     <t>Bảo trì máy móc thiết bị</t>
   </si>
   <si>
-    <t>BETA 4 (REACTJS-NODEJS)</t>
+    <t>BETA 4 (REACTJS - NODEJS)</t>
   </si>
   <si>
     <t>5,000,000</t>
@@ -435,7 +435,7 @@
     <t>Quản lý thương hiệu</t>
   </si>
   <si>
-    <t>BETA 2 (REACTJS-NODEJS)</t>
+    <t>BETA 2 (REACTJS - NODEJS)</t>
   </si>
   <si>
     <t>Quy trình mua hàng 26/9 L2</t>
@@ -498,7 +498,7 @@
     <t>Nâng cấp phần mềm quản lý kho</t>
   </si>
   <si>
-    <t>GAMMA (PYTHON-DJANGO)</t>
+    <t>GAMMA (PYTHON - DJANGO)</t>
   </si>
   <si>
     <t>Luồng báo giá hỏi nhà cung cấp 9/10 L2 [REQ_T9.2024_17]</t>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>Hợp đồng bảo trì định kỳ</t>
+  </si>
+  <si>
+    <t>DELTA (PHP - LARAVEL)</t>
   </si>
   <si>
     <t>Quy trình mua hàng 16/9 L1</t>
@@ -1959,10 +1962,10 @@
       <c r="F4" s="12">
         <v>0.4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="15" t="s">
         <v>64</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -2005,10 +2008,10 @@
       <c r="F5" s="12">
         <v>0.4</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="15" t="s">
         <v>70</v>
       </c>
       <c r="I5" s="15" t="s">
@@ -2235,10 +2238,10 @@
       <c r="F10" s="12">
         <v>0.9</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="15" t="s">
         <v>101</v>
       </c>
       <c r="I10" s="15" t="s">
@@ -2281,10 +2284,10 @@
       <c r="F11" s="12">
         <v>0.3</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="15" t="s">
         <v>105</v>
       </c>
       <c r="I11" s="15" t="s">
@@ -2327,10 +2330,10 @@
       <c r="F12" s="12">
         <v>0.8</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="15" t="s">
         <v>111</v>
       </c>
       <c r="I12" s="15" t="s">
@@ -2511,10 +2514,10 @@
       <c r="F16" s="12">
         <v>0.1</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="15" t="s">
         <v>111</v>
       </c>
       <c r="I16" s="15" t="s">
@@ -2557,10 +2560,10 @@
       <c r="F17" s="12">
         <v>0.8</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="15" t="s">
         <v>70</v>
       </c>
       <c r="I17" s="15" t="s">
@@ -2603,10 +2606,10 @@
       <c r="F18" s="12">
         <v>0.4</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="15" t="s">
         <v>101</v>
       </c>
       <c r="I18" s="15" t="s">
@@ -2833,10 +2836,10 @@
       <c r="F23" s="12">
         <v>0.6</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="15" t="s">
         <v>138</v>
       </c>
       <c r="I23" s="15" t="s">
@@ -3386,10 +3389,10 @@
         <v>0.4</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="I35" s="15" t="s">
         <v>79</v>
@@ -3407,7 +3410,7 @@
         <v>82</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O35" s="16"/>
     </row>
@@ -3417,7 +3420,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C36" s="14">
         <v>45580.0</v>
@@ -3453,7 +3456,7 @@
         <v>98</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O36" s="16"/>
     </row>
@@ -3463,7 +3466,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C37" s="14">
         <v>45581.0</v>
@@ -3499,7 +3502,7 @@
         <v>61</v>
       </c>
       <c r="N37" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O37" s="16"/>
     </row>
@@ -4504,7 +4507,7 @@
         <v>41</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D1" s="23"/>
       <c r="E1" s="24"/>
@@ -4513,13 +4516,13 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -4536,7 +4539,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -4554,7 +4557,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -4568,11 +4571,11 @@
       <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>15</v>
+      <c r="D5" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -4590,7 +4593,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -4604,11 +4607,11 @@
       <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>21</v>
+      <c r="D7" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -4626,7 +4629,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -4644,7 +4647,7 @@
         <v>23</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -4662,7 +4665,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -4680,7 +4683,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -4698,7 +4701,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -4716,7 +4719,7 @@
         <v>28</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -4734,7 +4737,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -4752,7 +4755,7 @@
         <v>28</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -4770,7 +4773,7 @@
         <v>33</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -4788,7 +4791,7 @@
         <v>18</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -4806,7 +4809,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -4824,7 +4827,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -4842,7 +4845,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -4860,7 +4863,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -4878,7 +4881,7 @@
         <v>12</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -4896,7 +4899,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -5921,54 +5924,54 @@
         <v>41</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F1" s="23"/>
       <c r="G1" s="24"/>
       <c r="H1" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" s="28" t="s">
         <v>192</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>191</v>
       </c>
       <c r="K1" s="23"/>
       <c r="L1" s="24"/>
       <c r="M1" s="27" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O1" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="P1" s="23"/>
       <c r="Q1" s="24"/>
       <c r="R1" s="27" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="S1" s="27" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="T1" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="U1" s="23"/>
       <c r="V1" s="24"/>
       <c r="W1" s="27" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="X1" s="27" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -5977,46 +5980,46 @@
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
       <c r="E2" s="27" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
       <c r="J2" s="27" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
       <c r="O2" s="27" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="R2" s="29"/>
       <c r="S2" s="29"/>
       <c r="T2" s="27" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U2" s="27" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V2" s="27" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="W2" s="29"/>
       <c r="X2" s="29"/>
@@ -6029,28 +6032,28 @@
         <v>54</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F3" s="30">
         <v>3.0</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="K3" s="30">
         <v>1.0</v>
@@ -6059,19 +6062,19 @@
         <v>98</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N3" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O3" s="30" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="P3" s="30">
         <v>6.0</v>
       </c>
       <c r="Q3" s="30" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="R3" s="31"/>
       <c r="S3" s="31"/>
@@ -6090,13 +6093,13 @@
         <v>63</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F4" s="30">
         <v>10.0</v>
@@ -6105,24 +6108,24 @@
         <v>75</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K4" s="30">
         <v>10.0</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M4" s="31"/>
       <c r="N4" s="31"/>
       <c r="O4" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="P4" s="30"/>
       <c r="Q4" s="30"/>
@@ -6143,13 +6146,13 @@
         <v>69</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F5" s="30">
         <v>6.0</v>
@@ -6158,24 +6161,24 @@
         <v>75</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K5" s="30">
         <v>7.0</v>
       </c>
       <c r="L5" s="30" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M5" s="31"/>
       <c r="N5" s="31"/>
       <c r="O5" s="17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="P5" s="30"/>
       <c r="Q5" s="30"/>
@@ -6196,13 +6199,13 @@
         <v>77</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F6" s="30">
         <v>1.0</v>
@@ -6211,24 +6214,24 @@
         <v>75</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K6" s="30">
         <v>5.0</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
       <c r="O6" s="17" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="P6" s="30"/>
       <c r="Q6" s="30"/>
@@ -6249,13 +6252,13 @@
         <v>84</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F7" s="30">
         <v>10.0</v>
@@ -6264,13 +6267,13 @@
         <v>75</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K7" s="30">
         <v>6.0</v>
@@ -6281,7 +6284,7 @@
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
       <c r="O7" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="P7" s="30"/>
       <c r="Q7" s="30"/>
@@ -6302,13 +6305,13 @@
         <v>89</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F8" s="30">
         <v>9.0</v>
@@ -6317,13 +6320,13 @@
         <v>75</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K8" s="30">
         <v>3.0</v>
@@ -6334,7 +6337,7 @@
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
       <c r="O8" s="17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="P8" s="30"/>
       <c r="Q8" s="31"/>
@@ -6355,13 +6358,13 @@
         <v>94</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F9" s="30">
         <v>3.0</v>
@@ -6370,13 +6373,13 @@
         <v>75</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K9" s="30">
         <v>5.0</v>
@@ -6386,7 +6389,7 @@
       </c>
       <c r="N9" s="31"/>
       <c r="O9" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="P9" s="30"/>
       <c r="Q9" s="31"/>
@@ -6407,13 +6410,13 @@
         <v>100</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F10" s="30">
         <v>7.0</v>
@@ -6422,24 +6425,24 @@
         <v>75</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K10" s="30">
         <v>8.0</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M10" s="31"/>
       <c r="N10" s="31"/>
       <c r="O10" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="31"/>
@@ -6460,13 +6463,13 @@
         <v>104</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F11" s="30">
         <v>2.0</v>
@@ -6475,28 +6478,28 @@
         <v>98</v>
       </c>
       <c r="H11" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="I11" s="30" t="s">
-        <v>220</v>
-      </c>
       <c r="J11" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K11" s="30">
         <v>8.0</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M11" s="30" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="N11" s="30" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P11" s="30">
         <v>1.0</v>
@@ -6521,28 +6524,28 @@
         <v>110</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F12" s="30">
         <v>7.0</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I12" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K12" s="30">
         <v>8.0</v>
@@ -6551,19 +6554,19 @@
         <v>98</v>
       </c>
       <c r="M12" s="30" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N12" s="30" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="P12" s="30">
         <v>5.0</v>
       </c>
       <c r="Q12" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="R12" s="31"/>
       <c r="S12" s="31"/>
@@ -6582,43 +6585,43 @@
         <v>114</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F13" s="30">
         <v>2.0</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K13" s="30">
         <v>4.0</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N13" s="30" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="P13" s="30">
         <v>8.0</v>
@@ -6643,43 +6646,43 @@
         <v>119</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F14" s="30">
         <v>1.0</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K14" s="30">
         <v>1.0</v>
       </c>
       <c r="L14" s="31" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M14" s="30" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N14" s="30" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="P14" s="30">
         <v>1.0</v>
@@ -6704,28 +6707,28 @@
         <v>122</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F15" s="30">
         <v>8.0</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K15" s="30">
         <v>7.0</v>
@@ -6734,13 +6737,13 @@
         <v>75</v>
       </c>
       <c r="M15" s="30" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N15" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P15" s="30">
         <v>4.0</v>
@@ -6765,28 +6768,28 @@
         <v>124</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F16" s="30">
         <v>2.0</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K16" s="30">
         <v>7.0</v>
@@ -6795,13 +6798,13 @@
         <v>75</v>
       </c>
       <c r="M16" s="30" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="N16" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="P16" s="30">
         <v>6.0</v>
@@ -6826,28 +6829,28 @@
         <v>127</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F17" s="30">
         <v>6.0</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I17" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K17" s="30">
         <v>5.0</v>
@@ -6856,13 +6859,13 @@
         <v>98</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N17" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="P17" s="30">
         <v>7.0</v>
@@ -6887,13 +6890,13 @@
         <v>129</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F18" s="30">
         <v>9.0</v>
@@ -6902,28 +6905,28 @@
         <v>75</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K18" s="30">
         <v>2.0</v>
       </c>
       <c r="L18" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M18" s="30" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="N18" s="30" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="P18" s="30">
         <v>1.0</v>
@@ -6948,13 +6951,13 @@
         <v>131</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F19" s="30">
         <v>6.0</v>
@@ -6963,28 +6966,28 @@
         <v>98</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K19" s="30">
         <v>1.0</v>
       </c>
       <c r="L19" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="M19" s="30" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="N19" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="P19" s="30">
         <v>9.0</v>
@@ -7009,43 +7012,43 @@
         <v>132</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F20" s="30">
         <v>4.0</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K20" s="30">
         <v>8.0</v>
       </c>
       <c r="L20" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M20" s="30" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N20" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="P20" s="30">
         <v>9.0</v>
@@ -7070,28 +7073,28 @@
         <v>134</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F21" s="30">
         <v>8.0</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I21" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K21" s="30">
         <v>4.0</v>
@@ -7100,19 +7103,19 @@
         <v>75</v>
       </c>
       <c r="M21" s="30" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N21" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P21" s="30">
         <v>10.0</v>
       </c>
       <c r="Q21" s="31" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="R21" s="31"/>
       <c r="S21" s="31"/>
@@ -7131,43 +7134,43 @@
         <v>135</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F22" s="30">
         <v>10.0</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K22" s="30">
         <v>3.0</v>
       </c>
       <c r="L22" s="31" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M22" s="30" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="N22" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="P22" s="30">
         <v>6.0</v>
@@ -7192,28 +7195,28 @@
         <v>137</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F23" s="30">
         <v>4.0</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I23" s="30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K23" s="30">
         <v>1.0</v>
@@ -7222,13 +7225,13 @@
         <v>98</v>
       </c>
       <c r="M23" s="30" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="P23" s="30">
         <v>7.0</v>

</xml_diff>